<commit_message>
implement stack adt, upload notes
</commit_message>
<xml_diff>
--- a/sorting_algorithms.xlsx
+++ b/sorting_algorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbildner/Desktop/AA-Data-Structures-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F787C5CA-538A-184A-BE3E-C5F3767BFD3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D0145A-76A5-9E4A-AEF9-6AB6F2DB0F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33460" windowHeight="28340" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14020" yWindow="460" windowWidth="33460" windowHeight="28340" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SelectionSort" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>Problem #</t>
   </si>
@@ -1788,6 +1788,18 @@
   </si>
   <si>
     <t>// 4) else exit loop (num &gt;= prev) bec now we know where to insert currentNum</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>Radix Sort</t>
+  </si>
+  <si>
+    <t>Counting Sort</t>
   </si>
 </sst>
 </file>
@@ -2683,7 +2695,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2994,7 +3006,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3343,10 +3355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3431,6 +3443,50 @@
         <v>32</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>912</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
implement stack ADT to solve LC20 valid parentheses
</commit_message>
<xml_diff>
--- a/sorting_algorithms.xlsx
+++ b/sorting_algorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbildner/Desktop/AA-Data-Structures-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D0145A-76A5-9E4A-AEF9-6AB6F2DB0F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C4D269-A487-A041-BFF5-B7E879B81F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="460" windowWidth="33460" windowHeight="28340" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8380" yWindow="460" windowWidth="33460" windowHeight="28340" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SelectionSort" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t>Problem #</t>
   </si>
@@ -1800,6 +1800,9 @@
   </si>
   <si>
     <t>Counting Sort</t>
+  </si>
+  <si>
+    <t>Side by side comparison sort</t>
   </si>
 </sst>
 </file>
@@ -3358,7 +3361,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3402,6 +3405,9 @@
       <c r="C2" s="1">
         <v>912</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="34" t="s">

</xml_diff>